<commit_message>
CIDC-1278 updates from Jen
</commit_message>
<xml_diff>
--- a/template_examples/tumor_tissue_rna_template.xlsx
+++ b/template_examples/tumor_tissue_rna_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" state="visible" r:id="rId2"/>
@@ -328,7 +328,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+          <t xml:space="preserve">Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as CTTTPPPSS.AA for trial code TTT, participant PPP, sample SS, and aliquot AA.</t>
         </r>
       </text>
     </comment>
@@ -659,12 +659,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4550" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4553" uniqueCount="288">
   <si>
     <t xml:space="preserve">#title</t>
   </si>
   <si>
-    <t xml:space="preserve">Shipping manifest for tissue dna extracted from tumor tissue samples</t>
+    <t xml:space="preserve">Biospecimen manifest for tumor tissue rna</t>
   </si>
   <si>
     <t xml:space="preserve">#preamble</t>
@@ -1123,7 +1123,7 @@
     <t xml:space="preserve">String: regex ^C[A-Z0-9]{3}[A-Z0-9]{3}[A-Z0-9]{2}.[0-9]{2}$ </t>
   </si>
   <si>
-    <t xml:space="preserve">Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+    <t xml:space="preserve">Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as CTTTPPPSS.AA for trial code TTT, participant PPP, sample SS, and aliquot AA.</t>
   </si>
   <si>
     <t xml:space="preserve">E.g. 'CTTTP01A1.00'</t>
@@ -1378,6 +1378,9 @@
     <t xml:space="preserve">Bone Marrow Mononuclear Cell</t>
   </si>
   <si>
+    <t xml:space="preserve">Stool DNA</t>
+  </si>
+  <si>
     <t xml:space="preserve">LN</t>
   </si>
   <si>
@@ -1426,85 +1429,91 @@
     <t xml:space="preserve">mIF</t>
   </si>
   <si>
+    <t xml:space="preserve">MSSM_MTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lumbar Puncture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H&amp;E-Stained Fixed Tissue Slide Specimen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mIHC</t>
+  </si>
+  <si>
     <t xml:space="preserve">DFCI_Wu</t>
   </si>
   <si>
-    <t xml:space="preserve">Stool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lumbar Puncture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H&amp;E-Stained Fixed Tissue Slide Specimen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mIHC</t>
+    <t xml:space="preserve">Cell Product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aspirate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCRseq</t>
   </si>
   <si>
     <t xml:space="preserve">DFCI_Hodi</t>
   </si>
   <si>
-    <t xml:space="preserve">Cell Product</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aspirate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCRseq</t>
+    <t xml:space="preserve">White Blood Cell Apheresis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fine-Needle Aspiration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tissue Scroll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATACseq</t>
   </si>
   <si>
     <t xml:space="preserve">DFCI_Severgnini</t>
   </si>
   <si>
-    <t xml:space="preserve">White Blood Cell Apheresis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fine-Needle Aspiration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tissue Scroll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATACseq</t>
+    <t xml:space="preserve">FFPE Punch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ctDNA</t>
   </si>
   <si>
     <t xml:space="preserve">DFCI_Livak</t>
   </si>
   <si>
-    <t xml:space="preserve">FFPE Punch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ctDNA</t>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microbiome</t>
   </si>
   <si>
     <t xml:space="preserve">Broad_Cibulskis</t>
   </si>
   <si>
-    <t xml:space="preserve">13</t>
+    <t xml:space="preserve">14</t>
   </si>
   <si>
     <t xml:space="preserve">Stanf_Maecker</t>
   </si>
   <si>
-    <t xml:space="preserve">14</t>
+    <t xml:space="preserve">15</t>
   </si>
   <si>
     <t xml:space="preserve">Stanf_Bendall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15</t>
   </si>
   <si>
     <t xml:space="preserve">NCH</t>
@@ -1751,8 +1760,8 @@
   </sheetPr>
   <dimension ref="A1:C2018"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B3:AE8 C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11961,8 +11970,8 @@
   </sheetPr>
   <dimension ref="A1:AE2002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:AE8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22662,7 +22671,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="R9:R2002" type="list">
-      <formula1>'Data Dictionary'!$M$2:$M$7</formula1>
+      <formula1>'Data Dictionary'!$M$2:$M$8</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="T9:T2002" type="list">
@@ -22717,7 +22726,7 @@
   <dimension ref="B1:E50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3:AE8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23322,10 +23331,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:U18"/>
+  <dimension ref="B1:U19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3:AE8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23669,7 +23678,7 @@
         <v>238</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>83</v>
+        <v>239</v>
       </c>
       <c r="O6" s="0" t="s">
         <v>83</v>
@@ -23681,7 +23690,7 @@
         <v>98</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="T6" s="0" t="s">
         <v>117</v>
@@ -23692,31 +23701,31 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>117</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="K7" s="0" t="s">
         <v>116</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="O7" s="0" t="s">
         <v>117</v>
@@ -23733,31 +23742,34 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="K8" s="0" t="s">
         <v>83</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>117</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="R8" s="0" t="s">
         <v>117</v>
@@ -23765,25 +23777,25 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="K9" s="0" t="s">
         <v>117</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="P9" s="0" t="s">
         <v>83</v>
@@ -23794,19 +23806,19 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L10" s="0" t="s">
         <v>75</v>
@@ -23820,33 +23832,33 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>83</v>
@@ -23855,18 +23867,18 @@
         <v>83</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>117</v>
@@ -23880,10 +23892,13 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>279</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="L14" s="0" t="s">
         <v>117</v>
@@ -23891,18 +23906,18 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23910,7 +23925,7 @@
         <v>83</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -23918,7 +23933,12 @@
         <v>117</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>284</v>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D19" s="0" t="s">
+        <v>287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>